<commit_message>
Fix - [Feature] Add new columns in cost export
</commit_message>
<xml_diff>
--- a/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/ExportProductCostList.xlsx
+++ b/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/ExportProductCostList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Produits" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,9 +13,9 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Coûts!$B$3:$E$3</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Produits!$B$3:$H$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Produits!$B$3:$K$3</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Produits!$B$3:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Coûts!$B$3:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Produits!$B$3:$H$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -27,84 +27,102 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
-  <si>
-    <t>TYPE</t>
-  </si>
-  <si>
-    <t>bcpg:product</t>
-  </si>
-  <si>
-    <t>COLUMNS</t>
-  </si>
-  <si>
-    <t>cm:name</t>
-  </si>
-  <si>
-    <t>bcpg:code</t>
-  </si>
-  <si>
-    <t>bcpg:erpCode</t>
-  </si>
-  <si>
-    <t>bcpg:productHierarchy1</t>
-  </si>
-  <si>
-    <t>bcpg:productHierarchy2</t>
-  </si>
-  <si>
-    <t>cm:description</t>
-  </si>
-  <si>
-    <t>bcpg:legalName</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>Nom</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Code ERP</t>
-  </si>
-  <si>
-    <t>Famille</t>
-  </si>
-  <si>
-    <t>Sous famille</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Libellé légal</t>
-  </si>
-  <si>
-    <t>bcpg:costList</t>
-  </si>
-  <si>
-    <t>bcpg:costListCost</t>
-  </si>
-  <si>
-    <t>bcpg:costListValue</t>
-  </si>
-  <si>
-    <t>bcpg:costListUnit</t>
-  </si>
-  <si>
-    <t>Produit</t>
-  </si>
-  <si>
-    <t>Coût</t>
-  </si>
-  <si>
-    <t>Valeur</t>
-  </si>
-  <si>
-    <t>Unité</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+  <si>
+    <t xml:space="preserve">TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLUMNS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cm:name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:erpCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:productHierarchy1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:productHierarchy2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cm:description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:legalName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:unitPrice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:priceCurrency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:unitTotalCost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code ERP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Famille</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sous famille</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Libellé légal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prix de vente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monnaie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coût de revient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:costList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:costListCost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:costListValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:costListUnit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Produit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coût</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valeur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unité</t>
   </si>
 </sst>
 </file>
@@ -112,7 +130,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -280,22 +298,23 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.75"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="8" style="0" width="11.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.1" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -331,38 +350,56 @@
       <c r="H2" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="I2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B3:H3"/>
+  <autoFilter ref="B3:K3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -379,14 +416,14 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.2602040816327"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="10.26"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -394,7 +431,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="7.45" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -405,37 +442,37 @@
         <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B3:E3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>

</xml_diff>